<commit_message>
update data and figure
</commit_message>
<xml_diff>
--- a/data/FPGA_chip.xlsx
+++ b/data/FPGA_chip.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>XC7Z020</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -38,15 +38,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>reg</t>
+    <t>5CEA7</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>sram</t>
+    <t>10AX115</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>5CSXC6</t>
+    <t>5SGXA7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SRAM</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -175,7 +183,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>reg</c:v>
+                  <c:v>REG</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -192,16 +200,25 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$D$1</c:f>
+              <c:f>Sheet1!$B$1:$G$1</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>XC7Z020</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>5CEA7</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>ZU9EG</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>5SGXA7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10AX115</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>VU9P</c:v>
                 </c:pt>
               </c:strCache>
@@ -209,17 +226,26 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$D$2</c:f>
+              <c:f>Sheet1!$B$2:$G$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>12.98828125</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>18.24951171875</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>66.9140625</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>114.609375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>208.59375</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>288.6328125</c:v>
                 </c:pt>
               </c:numCache>
@@ -240,7 +266,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>sram</c:v>
+                  <c:v>SRAM</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -257,16 +283,25 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$D$1</c:f>
+              <c:f>Sheet1!$B$1:$G$1</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>XC7Z020</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>5CEA7</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>ZU9EG</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>5SGXA7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10AX115</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>VU9P</c:v>
                 </c:pt>
               </c:strCache>
@@ -274,17 +309,26 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$D$3</c:f>
+              <c:f>Sheet1!$B$3:$G$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>630</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>857.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>4104</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>6400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6784</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>44280</c:v>
                 </c:pt>
               </c:numCache>
@@ -1041,16 +1085,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>628650</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1335,64 +1379,90 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
       </c>
       <c r="E1" t="s">
         <v>5</v>
       </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <f>106400/8/1024</f>
         <v>12.98828125</v>
       </c>
       <c r="C2">
+        <f>149500/8/1024</f>
+        <v>18.24951171875</v>
+      </c>
+      <c r="D2">
         <f>548160/8/1024</f>
         <v>66.9140625</v>
       </c>
-      <c r="D2">
+      <c r="E2">
+        <f>938880/8/1024</f>
+        <v>114.609375</v>
+      </c>
+      <c r="F2">
+        <f>1708800/1024/8</f>
+        <v>208.59375</v>
+      </c>
+      <c r="G2">
         <f>2364480/8/1024</f>
         <v>288.6328125</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <f>140*36/8</f>
         <v>630</v>
       </c>
       <c r="C3">
+        <f>6860/8</f>
+        <v>857.5</v>
+      </c>
+      <c r="D3">
         <f>912*36/8</f>
         <v>4104</v>
       </c>
-      <c r="D3">
+      <c r="E3">
+        <f>50*1024/8</f>
+        <v>6400</v>
+      </c>
+      <c r="F3">
+        <f>53*1024/8</f>
+        <v>6784</v>
+      </c>
+      <c r="G3">
         <f>2160*36/8+960*288/8</f>
         <v>44280</v>
-      </c>
-      <c r="E3">
-        <f>5570/8</f>
-        <v>696.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>